<commit_message>
update on categories and faculty
</commit_message>
<xml_diff>
--- a/public/Pinnit Accounts.xlsx
+++ b/public/Pinnit Accounts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richardluo/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00BA12F-DE6F-4643-A829-D2C07327EC6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2544856-C679-BD42-95A0-975416D65B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-100" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Faculties &amp; Programs" sheetId="1" r:id="rId1"/>
@@ -4379,7 +4379,7 @@
     <t>Fraternities &amp; Sororities</t>
   </si>
   <si>
-    <t>Varcity Clubs</t>
+    <t>Varsity Clubs</t>
   </si>
 </sst>
 </file>
@@ -4666,8 +4666,8 @@
   </sheetPr>
   <dimension ref="A1:E242"/>
   <sheetViews>
-    <sheetView topLeftCell="A211" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H228" sqref="H228"/>
+    <sheetView tabSelected="1" topLeftCell="A224" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E240" sqref="E240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9282,7 +9282,7 @@
   </sheetPr>
   <dimension ref="A1:E237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A209" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A172" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C241" sqref="C241"/>
     </sheetView>
   </sheetViews>

</xml_diff>